<commit_message>
adds structure to zeitprotokoll
</commit_message>
<xml_diff>
--- a/Zeitprotokoll.xlsx
+++ b/Zeitprotokoll.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qherren\Development\TBZ\M324\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92446E25-C6F9-4779-9034-BEE9C8432AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arbeitszeit" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +24,40 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>TaskNr</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Person(KG, NS, QH, SB)</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>QH</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,15 +67,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,15 +89,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +391,565 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.109375" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>